<commit_message>
updated after discussions with Kaite. Preppred for 30 Oct
</commit_message>
<xml_diff>
--- a/DNA/Extraction_MasterList.xlsx
+++ b/DNA/Extraction_MasterList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8685"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Sample_ID</t>
   </si>
   <si>
-    <t>Treatment</t>
-  </si>
-  <si>
     <t>Mass_g</t>
   </si>
   <si>
@@ -62,7 +59,64 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>RGF1</t>
+    <t>MT1</t>
+  </si>
+  <si>
+    <t>MT2</t>
+  </si>
+  <si>
+    <t>MT3</t>
+  </si>
+  <si>
+    <t>MT4</t>
+  </si>
+  <si>
+    <t>MT5</t>
+  </si>
+  <si>
+    <t>MT6</t>
+  </si>
+  <si>
+    <t>MT7</t>
+  </si>
+  <si>
+    <t>MT8</t>
+  </si>
+  <si>
+    <t>MT9</t>
+  </si>
+  <si>
+    <t>MT10</t>
+  </si>
+  <si>
+    <t>MT11</t>
+  </si>
+  <si>
+    <t>MT12</t>
+  </si>
+  <si>
+    <t>MT13</t>
+  </si>
+  <si>
+    <t>MT14</t>
+  </si>
+  <si>
+    <t>MT15</t>
+  </si>
+  <si>
+    <t>MT16</t>
+  </si>
+  <si>
+    <t>MT17</t>
+  </si>
+  <si>
+    <t>MT18</t>
+  </si>
+  <si>
+    <t>MT19</t>
+  </si>
+  <si>
+    <t>Blank</t>
   </si>
 </sst>
 </file>
@@ -98,8 +152,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,37 +435,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -428,46 +483,287 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C8">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C12">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C13">
         <v>12</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D7">
-        <v>6</v>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1">
+        <v>45960</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monta samples DNA extracted
</commit_message>
<xml_diff>
--- a/DNA/Extraction_MasterList.xlsx
+++ b/DNA/Extraction_MasterList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -104,19 +104,58 @@
     <t>MT15</t>
   </si>
   <si>
-    <t>MT16</t>
-  </si>
-  <si>
-    <t>MT17</t>
-  </si>
-  <si>
-    <t>MT18</t>
-  </si>
-  <si>
-    <t>MT19</t>
-  </si>
-  <si>
     <t>Blank</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Predrain_Blk1</t>
+  </si>
+  <si>
+    <t>Predrain_Blk2</t>
+  </si>
+  <si>
+    <t>Predrain_Blk3</t>
+  </si>
+  <si>
+    <t>B_1</t>
+  </si>
+  <si>
+    <t>Postreflood_101</t>
+  </si>
+  <si>
+    <t>Postreflood_103</t>
+  </si>
+  <si>
+    <t>Postreflood_201</t>
+  </si>
+  <si>
+    <t>Postreflood_202</t>
+  </si>
+  <si>
+    <t>Postreflood_301</t>
+  </si>
+  <si>
+    <t>Postreflood_303</t>
+  </si>
+  <si>
+    <t>Late_ 101</t>
+  </si>
+  <si>
+    <t>Late_ 103</t>
+  </si>
+  <si>
+    <t>Late_ 201</t>
+  </si>
+  <si>
+    <t>Late_ 202</t>
+  </si>
+  <si>
+    <t>Late_ 301</t>
+  </si>
+  <si>
+    <t>Late_ 303</t>
   </si>
 </sst>
 </file>
@@ -132,15 +171,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -148,13 +193,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,338 +498,472 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E2" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E3" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="E4" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D5" s="2">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E5" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D6" s="2">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E6" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D7" s="2">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="E7" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D8" s="2">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E8" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D9" s="2">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D10" s="2">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="E10" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D11" s="2">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="E11" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D12" s="2">
         <v>11</v>
       </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E12" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C13">
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D13" s="2">
         <v>12</v>
       </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="E13" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D14" s="2">
         <v>13</v>
       </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E14" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D15" s="2">
         <v>14</v>
       </c>
-      <c r="E15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E15" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D16" s="2">
         <v>15</v>
       </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E16" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C17">
+      <c r="C17" s="3">
+        <v>45967</v>
+      </c>
+      <c r="D17" s="2">
         <v>16</v>
       </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C18">
-        <v>17</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C19">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C20">
-        <v>19</v>
-      </c>
-      <c r="E20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="1">
-        <v>45960</v>
-      </c>
-      <c r="C21">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>8</v>
-      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added in oven dry total biomass weights
</commit_message>
<xml_diff>
--- a/DNA/Extraction_MasterList.xlsx
+++ b/DNA/Extraction_MasterList.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8688" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="6_Nov_2025" sheetId="1" r:id="rId1"/>
+    <sheet name="14_Nov_2025" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="135">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -156,6 +157,279 @@
   </si>
   <si>
     <t>Late_ 303</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>S19</t>
+  </si>
+  <si>
+    <t>S20</t>
+  </si>
+  <si>
+    <t>S21</t>
+  </si>
+  <si>
+    <t>S22</t>
+  </si>
+  <si>
+    <t>S23</t>
+  </si>
+  <si>
+    <t>S24</t>
+  </si>
+  <si>
+    <t>S25</t>
+  </si>
+  <si>
+    <t>S26</t>
+  </si>
+  <si>
+    <t>S27</t>
+  </si>
+  <si>
+    <t>S28</t>
+  </si>
+  <si>
+    <t>S29</t>
+  </si>
+  <si>
+    <t>S30</t>
+  </si>
+  <si>
+    <t>S31</t>
+  </si>
+  <si>
+    <t>S32</t>
+  </si>
+  <si>
+    <t>S33</t>
+  </si>
+  <si>
+    <t>S34</t>
+  </si>
+  <si>
+    <t>S35</t>
+  </si>
+  <si>
+    <t>S36</t>
+  </si>
+  <si>
+    <t>S37</t>
+  </si>
+  <si>
+    <t>S38</t>
+  </si>
+  <si>
+    <t>S39</t>
+  </si>
+  <si>
+    <t>S40</t>
+  </si>
+  <si>
+    <t>S41</t>
+  </si>
+  <si>
+    <t>S42</t>
+  </si>
+  <si>
+    <t>S43</t>
+  </si>
+  <si>
+    <t>S44</t>
+  </si>
+  <si>
+    <t>S45</t>
+  </si>
+  <si>
+    <t>S46</t>
+  </si>
+  <si>
+    <t>S47</t>
+  </si>
+  <si>
+    <t>101_Predrain</t>
+  </si>
+  <si>
+    <t>102_Predrain</t>
+  </si>
+  <si>
+    <t>103_Predrain</t>
+  </si>
+  <si>
+    <t>105_Predrain</t>
+  </si>
+  <si>
+    <t>106_Predrain</t>
+  </si>
+  <si>
+    <t>201_Predrain</t>
+  </si>
+  <si>
+    <t>203_Predrain</t>
+  </si>
+  <si>
+    <t>204_Predrain</t>
+  </si>
+  <si>
+    <t>205_Predrain</t>
+  </si>
+  <si>
+    <t>206_Predrain</t>
+  </si>
+  <si>
+    <t>301_Predrain</t>
+  </si>
+  <si>
+    <t>302_Predrain</t>
+  </si>
+  <si>
+    <t>304_Predrain</t>
+  </si>
+  <si>
+    <t>305_Predrain</t>
+  </si>
+  <si>
+    <t>306_Predrain</t>
+  </si>
+  <si>
+    <t>101_Post reflood</t>
+  </si>
+  <si>
+    <t>102_Post reflood</t>
+  </si>
+  <si>
+    <t>103_Post reflood</t>
+  </si>
+  <si>
+    <t>105_Post reflood</t>
+  </si>
+  <si>
+    <t>106_Post reflood</t>
+  </si>
+  <si>
+    <t>201_Post reflood</t>
+  </si>
+  <si>
+    <t>203_Post reflood</t>
+  </si>
+  <si>
+    <t>204_Post reflood</t>
+  </si>
+  <si>
+    <t>205_Post reflood</t>
+  </si>
+  <si>
+    <t>206_Post reflood</t>
+  </si>
+  <si>
+    <t>301_Post reflood</t>
+  </si>
+  <si>
+    <t>302_Post reflood</t>
+  </si>
+  <si>
+    <t>304_Post reflood</t>
+  </si>
+  <si>
+    <t>305_Post reflood</t>
+  </si>
+  <si>
+    <t>306_Post reflood</t>
+  </si>
+  <si>
+    <t>101_Late</t>
+  </si>
+  <si>
+    <t>102_Late</t>
+  </si>
+  <si>
+    <t>103_Late</t>
+  </si>
+  <si>
+    <t>105_Late</t>
+  </si>
+  <si>
+    <t>106_Late</t>
+  </si>
+  <si>
+    <t>201_Late</t>
+  </si>
+  <si>
+    <t>203_Late</t>
+  </si>
+  <si>
+    <t>204_Late</t>
+  </si>
+  <si>
+    <t>205_Late</t>
+  </si>
+  <si>
+    <t>206_Late</t>
+  </si>
+  <si>
+    <t>301_Late</t>
+  </si>
+  <si>
+    <t>302_Late</t>
+  </si>
+  <si>
+    <t>304_Late</t>
+  </si>
+  <si>
+    <t>305_Late</t>
+  </si>
+  <si>
+    <t>306_Late</t>
+  </si>
+  <si>
+    <t>B_2</t>
   </si>
 </sst>
 </file>
@@ -500,25 +774,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -553,7 +827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -578,7 +852,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -603,7 +877,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -628,7 +902,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -653,7 +927,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -678,7 +952,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -703,7 +977,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -728,7 +1002,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -753,7 +1027,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -778,7 +1052,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -803,7 +1077,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -828,7 +1102,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -853,7 +1127,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -878,7 +1152,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -903,7 +1177,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -928,7 +1202,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -953,14 +1227,1170 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D5" s="2">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D6" s="2">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D8" s="2">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D9" s="2">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D10" s="2">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D11" s="2">
+        <v>12</v>
+      </c>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D12" s="2">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D13" s="2">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D14" s="2">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D15" s="2">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D16" s="2">
+        <v>17</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D17" s="2">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D18" s="2">
+        <v>19</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D19" s="2">
+        <v>20</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D20" s="2">
+        <v>21</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D21" s="2">
+        <v>22</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D22" s="2">
+        <v>23</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D23" s="2">
+        <v>24</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D24" s="2">
+        <v>25</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D25" s="2">
+        <v>26</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D31" s="2">
+        <v>27</v>
+      </c>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C32" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D32" s="2">
+        <v>28</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D33" s="2">
+        <v>29</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D34" s="2">
+        <v>30</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D35" s="2">
+        <v>31</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D36" s="2">
+        <v>32</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D37" s="2">
+        <v>33</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D38" s="2">
+        <v>34</v>
+      </c>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D39" s="2">
+        <v>35</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D40" s="2">
+        <v>36</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D41" s="2">
+        <v>37</v>
+      </c>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D42" s="2">
+        <v>38</v>
+      </c>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D43" s="2">
+        <v>39</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C44" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D44" s="2">
+        <v>40</v>
+      </c>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D45" s="2">
+        <v>41</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C46" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D46" s="2">
+        <v>42</v>
+      </c>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D47" s="2">
+        <v>43</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D48" s="2">
+        <v>44</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C49" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D49" s="2">
+        <v>45</v>
+      </c>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D50" s="2">
+        <v>46</v>
+      </c>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D51" s="2">
+        <v>47</v>
+      </c>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="3">
+        <v>45975</v>
+      </c>
+      <c r="D52" s="2">
+        <v>48</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added trial extraction (for purification testing)
</commit_message>
<xml_diff>
--- a/DNA/Extraction_MasterList.xlsx
+++ b/DNA/Extraction_MasterList.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8688" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8685" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="6_Nov_2025" sheetId="1" r:id="rId1"/>
     <sheet name="14_Nov_2025" sheetId="3" r:id="rId2"/>
+    <sheet name="20_Nov_2025" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="139">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -51,9 +52,6 @@
     <t>Extraction_Date</t>
   </si>
   <si>
-    <t>EB</t>
-  </si>
-  <si>
     <t>Extraction_Num</t>
   </si>
   <si>
@@ -430,6 +428,21 @@
   </si>
   <si>
     <t>B_2</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test_Soils </t>
+  </si>
+  <si>
+    <t>For testing purification kits</t>
   </si>
 </sst>
 </file>
@@ -775,35 +788,35 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -824,15 +837,15 @@
         <v>6</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3">
         <v>45967</v>
@@ -844,7 +857,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -852,12 +865,12 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3">
         <v>45967</v>
@@ -869,7 +882,7 @@
         <v>0.38</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -877,12 +890,12 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="3">
         <v>45967</v>
@@ -894,7 +907,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -902,12 +915,12 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3">
         <v>45967</v>
@@ -919,7 +932,7 @@
         <v>0.37</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -927,12 +940,12 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3">
         <v>45967</v>
@@ -944,7 +957,7 @@
         <v>0.45</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -952,12 +965,12 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="3">
         <v>45967</v>
@@ -969,7 +982,7 @@
         <v>0.46</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -977,12 +990,12 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3">
         <v>45967</v>
@@ -994,7 +1007,7 @@
         <v>0.37</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1002,12 +1015,12 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="3">
         <v>45967</v>
@@ -1019,7 +1032,7 @@
         <v>0.39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1027,12 +1040,12 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="3">
         <v>45967</v>
@@ -1044,7 +1057,7 @@
         <v>0.47</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1052,12 +1065,12 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3">
         <v>45967</v>
@@ -1069,7 +1082,7 @@
         <v>0.56999999999999995</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1077,12 +1090,12 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="3">
         <v>45967</v>
@@ -1094,7 +1107,7 @@
         <v>0.43</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1102,12 +1115,12 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3">
         <v>45967</v>
@@ -1119,7 +1132,7 @@
         <v>0.43</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1127,12 +1140,12 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3">
         <v>45967</v>
@@ -1144,7 +1157,7 @@
         <v>0.46</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1152,12 +1165,12 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="3">
         <v>45967</v>
@@ -1169,7 +1182,7 @@
         <v>0.47</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1177,12 +1190,12 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3">
         <v>45967</v>
@@ -1194,7 +1207,7 @@
         <v>0.4</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1202,12 +1215,12 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="3">
         <v>45967</v>
@@ -1219,7 +1232,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1227,13 +1240,13 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
     </row>
   </sheetData>
@@ -1246,36 +1259,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K25"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:K56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -1296,15 +1309,15 @@
         <v>6</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3">
         <v>45975</v>
@@ -1314,7 +1327,7 @@
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -1322,12 +1335,12 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="3">
         <v>45975</v>
@@ -1337,7 +1350,7 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -1345,12 +1358,12 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="3">
         <v>45975</v>
@@ -1360,7 +1373,7 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -1368,12 +1381,12 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="3">
         <v>45975</v>
@@ -1383,7 +1396,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -1391,12 +1404,12 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="3">
         <v>45975</v>
@@ -1406,7 +1419,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -1414,12 +1427,12 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="3">
         <v>45975</v>
@@ -1429,7 +1442,7 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1437,12 +1450,12 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="3">
         <v>45975</v>
@@ -1452,7 +1465,7 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -1460,12 +1473,12 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9" s="3">
         <v>45975</v>
@@ -1475,7 +1488,7 @@
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -1483,12 +1496,12 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="3">
         <v>45975</v>
@@ -1498,7 +1511,7 @@
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1506,12 +1519,12 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="3">
         <v>45975</v>
@@ -1521,7 +1534,7 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1529,12 +1542,12 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" s="3">
         <v>45975</v>
@@ -1544,7 +1557,7 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1552,12 +1565,12 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="3">
         <v>45975</v>
@@ -1567,7 +1580,7 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1575,12 +1588,12 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="3">
         <v>45975</v>
@@ -1590,7 +1603,7 @@
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -1598,12 +1611,12 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" s="3">
         <v>45975</v>
@@ -1613,7 +1626,7 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -1621,12 +1634,12 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="3">
         <v>45975</v>
@@ -1636,7 +1649,7 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1644,12 +1657,12 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="3">
         <v>45975</v>
@@ -1659,7 +1672,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1667,12 +1680,12 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" s="3">
         <v>45975</v>
@@ -1682,7 +1695,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1690,12 +1703,12 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="3">
         <v>45975</v>
@@ -1705,7 +1718,7 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -1713,12 +1726,12 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C20" s="3">
         <v>45975</v>
@@ -1728,7 +1741,7 @@
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -1736,12 +1749,12 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" s="3">
         <v>45975</v>
@@ -1751,7 +1764,7 @@
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -1759,12 +1772,12 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C22" s="3">
         <v>45975</v>
@@ -1774,7 +1787,7 @@
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -1782,12 +1795,12 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C23" s="3">
         <v>45975</v>
@@ -1797,7 +1810,7 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1805,12 +1818,12 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C24" s="3">
         <v>45975</v>
@@ -1820,7 +1833,7 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1828,12 +1841,12 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25" s="3">
         <v>45975</v>
@@ -1843,7 +1856,7 @@
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -1851,18 +1864,18 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>1</v>
@@ -1883,15 +1896,15 @@
         <v>6</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C31" s="3">
         <v>45975</v>
@@ -1901,7 +1914,7 @@
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -1909,12 +1922,12 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C32" s="3">
         <v>45975</v>
@@ -1924,7 +1937,7 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
@@ -1932,12 +1945,12 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C33" s="3">
         <v>45975</v>
@@ -1947,7 +1960,7 @@
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -1955,12 +1968,12 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C34" s="3">
         <v>45975</v>
@@ -1970,7 +1983,7 @@
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -1978,12 +1991,12 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C35" s="3">
         <v>45975</v>
@@ -1993,7 +2006,7 @@
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
@@ -2001,12 +2014,12 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C36" s="3">
         <v>45975</v>
@@ -2016,7 +2029,7 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -2024,12 +2037,12 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C37" s="3">
         <v>45975</v>
@@ -2039,7 +2052,7 @@
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2047,12 +2060,12 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C38" s="3">
         <v>45975</v>
@@ -2062,7 +2075,7 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -2070,12 +2083,12 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C39" s="3">
         <v>45975</v>
@@ -2085,7 +2098,7 @@
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -2093,12 +2106,12 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C40" s="3">
         <v>45975</v>
@@ -2108,7 +2121,7 @@
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -2116,12 +2129,12 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C41" s="3">
         <v>45975</v>
@@ -2131,7 +2144,7 @@
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -2139,12 +2152,12 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C42" s="3">
         <v>45975</v>
@@ -2154,7 +2167,7 @@
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -2162,12 +2175,12 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C43" s="3">
         <v>45975</v>
@@ -2177,7 +2190,7 @@
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -2185,12 +2198,12 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C44" s="3">
         <v>45975</v>
@@ -2200,7 +2213,7 @@
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2208,12 +2221,12 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C45" s="3">
         <v>45975</v>
@@ -2223,7 +2236,7 @@
       </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -2231,12 +2244,12 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="3">
         <v>45975</v>
@@ -2246,7 +2259,7 @@
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -2254,12 +2267,12 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47" s="3">
         <v>45975</v>
@@ -2269,7 +2282,7 @@
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2277,12 +2290,12 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C48" s="3">
         <v>45975</v>
@@ -2292,7 +2305,7 @@
       </c>
       <c r="E48" s="2"/>
       <c r="F48" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
@@ -2300,12 +2313,12 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C49" s="3">
         <v>45975</v>
@@ -2315,7 +2328,7 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
@@ -2323,12 +2336,12 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C50" s="3">
         <v>45975</v>
@@ -2338,7 +2351,7 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -2346,12 +2359,12 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C51" s="3">
         <v>45975</v>
@@ -2361,7 +2374,7 @@
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -2369,12 +2382,12 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C52" s="3">
         <v>45975</v>
@@ -2384,7 +2397,7 @@
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>8</v>
+        <v>134</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -2396,4 +2409,132 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45981</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="2">
+        <v>53.2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1.87</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="J2" s="2">
+        <v>100</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45981</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="2">
+        <v>45.7</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.92</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="J3" s="2">
+        <v>100</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added zymo test run
</commit_message>
<xml_diff>
--- a/DNA/Extraction_MasterList.xlsx
+++ b/DNA/Extraction_MasterList.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhang\Documents\GitHub\Sulfate_Drain\DNA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE8F26F-BA31-4608-939C-65CB3324CBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8685" activeTab="2"/>
+    <workbookView xWindow="14303" yWindow="-907" windowWidth="21795" windowHeight="12974" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6_Nov_2025" sheetId="1" r:id="rId1"/>
     <sheet name="14_Nov_2025" sheetId="3" r:id="rId2"/>
     <sheet name="20_Nov_2025" sheetId="4" r:id="rId3"/>
+    <sheet name="23_Feb_2026" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="152">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -443,12 +445,51 @@
   </si>
   <si>
     <t>For testing purification kits</t>
+  </si>
+  <si>
+    <t>Kit</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Zymo-10</t>
+  </si>
+  <si>
+    <t>Zymo-5</t>
+  </si>
+  <si>
+    <t>DNA_Elution</t>
+  </si>
+  <si>
+    <t>We will proceed with this kit</t>
+  </si>
+  <si>
+    <t>Final incubation step was short, but should not have affected QC</t>
+  </si>
+  <si>
+    <t>These are from Zymo Research, Genomic DNA Clean &amp; Concentrator</t>
+  </si>
+  <si>
+    <t>10 is optimised for 10-50 kb</t>
+  </si>
+  <si>
+    <t>5 is optimised for 5 kb</t>
+  </si>
+  <si>
+    <t>Jessica noted that nanodrop may be going crazy LOL</t>
+  </si>
+  <si>
+    <t>Seems like the 260/280 value is a little high</t>
+  </si>
+  <si>
+    <t>I feel like 260 may be over predicted?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -784,11 +825,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,10 +1297,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="A54" sqref="A54:K56"/>
     </sheetView>
   </sheetViews>
@@ -2412,11 +2453,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2471,8 +2512,8 @@
       <c r="B2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="2">
-        <v>45981</v>
+      <c r="C2" s="3">
+        <v>46346</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -2506,8 +2547,8 @@
       <c r="B3" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="2">
-        <v>45981</v>
+      <c r="C3" s="3">
+        <v>46346</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -2532,6 +2573,278 @@
       </c>
       <c r="K3" s="2" t="s">
         <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16EADA40-7F92-4D45-93C7-8C343B372E2B}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="59.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="3">
+        <v>45981</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" s="2">
+        <v>53.2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.87</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="I2" s="2">
+        <v>99</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" s="3">
+        <v>45981</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45.7</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.92</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="I3" s="2">
+        <v>99</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="3">
+        <v>46076</v>
+      </c>
+      <c r="D4" s="2">
+        <v>38.4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="2">
+        <v>38.4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.27</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2.68</v>
+      </c>
+      <c r="I4" s="2">
+        <v>50</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="3">
+        <v>46076</v>
+      </c>
+      <c r="D5" s="2">
+        <v>40.9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="2">
+        <v>40.9</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2.31</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.98</v>
+      </c>
+      <c r="I5" s="2">
+        <v>50</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="3">
+        <v>46076</v>
+      </c>
+      <c r="D6" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="2">
+        <v>30.3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="I6" s="2">
+        <v>50</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="3">
+        <v>46076</v>
+      </c>
+      <c r="D7" s="2">
+        <v>25.9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="2">
+        <v>25.9</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.23</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="I7" s="2">
+        <v>50</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>